<commit_message>
Added quotes tables to the carpenter's list of tables scripted by sexy. This led to enabling interface based table rows to be marshalled to Sexy in GetRow methods.
</commit_message>
<xml_diff>
--- a/tables/quotes-table.xlsx
+++ b/tables/quotes-table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\rococo\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F22F037-AB14-4A47-BA3E-F2C8EAE75E97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413126F2-9AE7-48DA-9849-BEC04F665184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="4" xr2:uid="{00195B25-CB3D-43E0-A5F7-350564E66F68}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{00195B25-CB3D-43E0-A5F7-350564E66F68}"/>
   </bookViews>
   <sheets>
     <sheet name="Sexcel-Spec" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
   <si>
     <t>string</t>
   </si>
@@ -159,6 +159,12 @@
   </si>
   <si>
     <t>IQuotes</t>
+  </si>
+  <si>
+    <t>Sexy Header</t>
+  </si>
+  <si>
+    <t>tables\rococo.tables.test.sxh</t>
   </si>
 </sst>
 </file>
@@ -648,7 +654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3230684E-8A11-41FB-8526-9EA18FC7052C}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -723,10 +729,10 @@
   <sheetPr>
     <tabColor theme="6" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,6 +820,14 @@
         <v>36</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>